<commit_message>
🎨 add briding site form
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/oncho_3_dbs.xlsx
+++ b/ONCHO/OEM/oncho_3_dbs.xlsx
@@ -145,9 +145,6 @@
     <t>Sélectionner un district (UI)</t>
   </si>
   <si>
-    <t>p_RecorderID</t>
-  </si>
-  <si>
     <t>Select District</t>
   </si>
   <si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>O código é um número de dígitos entre 9 e 91</t>
+  </si>
+  <si>
+    <t>d_RecorderID</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P4" sqref="P4:P5"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -748,10 +748,10 @@
         <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -766,7 +766,7 @@
         <v>22</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>8</v>
@@ -778,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>11</v>
@@ -789,7 +789,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -804,10 +804,10 @@
         <v>36</v>
       </c>
       <c r="G2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="11" t="s">
@@ -820,7 +820,7 @@
         <v>33</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
@@ -835,10 +835,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
@@ -846,7 +846,7 @@
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="12"/>
@@ -867,18 +867,18 @@
         <v>28</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="12"/>
@@ -896,21 +896,21 @@
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>57</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -931,7 +931,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -955,7 +955,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1012,7 +1012,7 @@
         <v>18</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1105,10 +1105,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>20200406</v>

</xml_diff>